<commit_message>
infographic kca 2022 done
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\podesscript\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF09CE3-5736-4C3B-A903-0FB0DA26A247}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9B7C49-6D32-44BB-A139-3515625BB719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T1" sheetId="1" r:id="rId1"/>
@@ -60,6 +60,16 @@
     <definedName name="_xlnm.Print_Area" localSheetId="28">'T29'!$A$1:$F$12</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2737,7 +2747,7 @@
     <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314998" right="0.59055118110236204" top="0.78740157480314998" bottom="0.78740157480314998" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="11" scale="97" orientation="portrait" r:id="rId1"/>
   <headerFooter differentOddEven="1">
     <oddHeader>&amp;R&amp;"Calibri,Regular"&amp;10NAMA BAB</oddHeader>
     <oddFooter>&amp;R&amp;10Kecamatan XXX Dalam Angka 2020  |   &amp;P</oddFooter>
@@ -5668,8 +5678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5824,7 +5834,7 @@
     <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314998" right="0.59055118110236204" top="0.78740157480314998" bottom="0.78740157480314998" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="11" scale="91" orientation="portrait" r:id="rId1"/>
   <headerFooter differentOddEven="1">
     <oddHeader>&amp;R&amp;"Calibri,Regular"&amp;10NAMA BAB</oddHeader>
     <oddFooter>&amp;R&amp;10Kecamatan XXX Dalam Angka 2020  |   &amp;P</oddFooter>
@@ -5839,7 +5849,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6015,7 +6025,7 @@
     <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314998" right="0.59055118110236204" top="0.78740157480314998" bottom="0.78740157480314998" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="11" scale="91" orientation="portrait" r:id="rId1"/>
   <headerFooter differentOddEven="1">
     <oddHeader>&amp;R&amp;"Calibri,Regular"&amp;10NAMA BAB</oddHeader>
     <oddFooter>&amp;R&amp;10Kecamatan XXX Dalam Angka 2020  |   &amp;P</oddFooter>
@@ -6190,8 +6200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6375,7 +6385,7 @@
     <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314998" right="0.59055118110236204" top="0.78740157480314998" bottom="0.78740157480314998" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="11" scale="87" orientation="portrait" r:id="rId1"/>
   <headerFooter differentOddEven="1">
     <oddHeader>&amp;R&amp;"Calibri,Regular"&amp;10NAMA BAB</oddHeader>
     <oddFooter>&amp;R&amp;10Kecamatan XXX Dalam Angka 2020  |   &amp;P</oddFooter>
@@ -6390,7 +6400,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6700,7 +6710,7 @@
     <mergeCell ref="A8:D8"/>
   </mergeCells>
   <pageMargins left="0.78740157480314998" right="0.59055118110236204" top="0.78740157480314998" bottom="0.78740157480314998" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="11" scale="89" orientation="portrait" r:id="rId1"/>
   <headerFooter differentOddEven="1">
     <oddHeader>&amp;R&amp;"Calibri,Regular"&amp;10NAMA BAB</oddHeader>
     <oddFooter>&amp;R&amp;10Kecamatan XXX Dalam Angka 2020  |   &amp;P</oddFooter>
@@ -6715,7 +6725,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6908,7 +6918,7 @@
     <mergeCell ref="C11:F11"/>
   </mergeCells>
   <pageMargins left="0.78740157480314998" right="0.59055118110236204" top="0.78740157480314998" bottom="0.78740157480314998" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="11" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="11" scale="98" orientation="portrait" r:id="rId1"/>
   <headerFooter differentOddEven="1">
     <oddHeader>&amp;R&amp;"Calibri,Regular"&amp;10NAMA BAB</oddHeader>
     <oddFooter>&amp;R&amp;10Kecamatan XXX Dalam Angka 2020  |   &amp;P</oddFooter>
@@ -6923,7 +6933,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7133,7 +7143,7 @@
     <mergeCell ref="C11:F11"/>
   </mergeCells>
   <pageMargins left="0.78740157480314998" right="0.59055118110236204" top="0.78740157480314998" bottom="0.78740157480314998" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="11" scale="93" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="11" scale="80" orientation="portrait" r:id="rId1"/>
   <headerFooter differentOddEven="1">
     <oddHeader>&amp;R&amp;"Calibri,Regular"&amp;10NAMA BAB</oddHeader>
     <oddFooter>&amp;R&amp;10Kecamatan XXX Dalam Angka 2020  |   &amp;P</oddFooter>
@@ -7147,8 +7157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>